<commit_message>
Proj2.c - run implemented | Error
</commit_message>
<xml_diff>
--- a/Project1/opcodes_proj1.xlsx
+++ b/Project1/opcodes_proj1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\윤태웅\Programming\Practice\20-1 Computer Architecture\Project1\Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA440192-CADC-4446-A48E-665AFB617FB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A160DBF9-080F-43D8-9052-23087AF6B747}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{65AC1469-6BCE-4854-8E69-3D40F6FA4BEE}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -860,14 +859,15 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15.19921875" customWidth="1"/>
     <col min="2" max="2" width="34.09765625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="16.296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>